<commit_message>
change order of spreadsheet
</commit_message>
<xml_diff>
--- a/config/initializers/spreadsheet_template.xlsx
+++ b/config/initializers/spreadsheet_template.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14720" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14720" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Dashboard" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Congratulations! This is your dashboard.</t>
   </si>
@@ -37,13 +37,16 @@
     <t>Item</t>
   </si>
   <si>
-    <t>Total Cost</t>
-  </si>
-  <si>
     <t>Description</t>
   </si>
   <si>
     <t>Please modify this worksheet and create new ones. But make sure to leave the "data" worksheet alone, unless you really know what you are doing.</t>
+  </si>
+  <si>
+    <t>Price</t>
+  </si>
+  <si>
+    <t>Amount</t>
   </si>
 </sst>
 </file>
@@ -94,7 +97,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -113,10 +116,13 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -452,7 +458,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
@@ -492,7 +498,7 @@
     </row>
     <row r="5" spans="1:20" ht="12.75" customHeight="1">
       <c r="A5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -507,38 +513,58 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:V1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B1" sqref="B1:B1048576"/>
+      <selection pane="bottomLeft" activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.1640625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="26.1640625" style="3" customWidth="1"/>
-    <col min="2" max="2" width="24.5" style="7" customWidth="1"/>
+    <col min="2" max="2" width="24.5" style="6" customWidth="1"/>
     <col min="3" max="3" width="29.83203125" customWidth="1"/>
     <col min="4" max="4" width="12.5" style="5" customWidth="1"/>
-    <col min="5" max="5" width="35.83203125" customWidth="1"/>
+    <col min="5" max="5" width="8.6640625" customWidth="1"/>
+    <col min="6" max="6" width="38.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="12.75" customHeight="1">
+    <row r="1" spans="1:22" ht="12.75" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="7" t="s">
         <v>4</v>
       </c>
       <c r="D1" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>6</v>
-      </c>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
+      <c r="I1" s="7"/>
+      <c r="J1" s="7"/>
+      <c r="K1" s="7"/>
+      <c r="L1" s="7"/>
+      <c r="M1" s="7"/>
+      <c r="N1" s="7"/>
+      <c r="O1" s="7"/>
+      <c r="P1" s="7"/>
+      <c r="Q1" s="7"/>
+      <c r="R1" s="7"/>
+      <c r="S1" s="7"/>
+      <c r="T1" s="7"/>
+      <c r="U1" s="7"/>
+      <c r="V1" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>